<commit_message>
Fixes a workflow bug
</commit_message>
<xml_diff>
--- a/custom-lens/tools/cloud-foundations-accelerator-workbook.xlsx
+++ b/custom-lens/tools/cloud-foundations-accelerator-workbook.xlsx
@@ -2284,7 +2284,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2493,12 +2493,8 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>379</v>
-      </c>
+      <c r="A13" s="3"/>
+      <c r="B13" s="4"/>
       <c r="C13" s="5" t="s">
         <v>397</v>
       </c>
@@ -2577,8 +2573,12 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
+      <c r="A18" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>380</v>
+      </c>
       <c r="C18" s="5" t="s">
         <v>402</v>
       </c>
@@ -2590,12 +2590,8 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>380</v>
-      </c>
+      <c r="A19" s="3"/>
+      <c r="B19" s="4"/>
       <c r="C19" s="5" t="s">
         <v>403</v>
       </c>
@@ -2608,10 +2604,10 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="3" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>404</v>
@@ -2637,12 +2633,8 @@
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>381</v>
-      </c>
+      <c r="A22" s="3"/>
+      <c r="B22" s="4"/>
       <c r="C22" s="5" t="s">
         <v>406</v>
       </c>
@@ -2654,12 +2646,8 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>381</v>
-      </c>
+      <c r="A23" s="3"/>
+      <c r="B23" s="4"/>
       <c r="C23" s="5" t="s">
         <v>407</v>
       </c>
@@ -2671,8 +2659,12 @@
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="3"/>
-      <c r="B24" s="4"/>
+      <c r="A24" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>382</v>
+      </c>
       <c r="C24" s="5" t="s">
         <v>408</v>
       </c>
@@ -2730,12 +2722,8 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="3" t="s">
-        <v>374</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>382</v>
-      </c>
+      <c r="A28" s="3"/>
+      <c r="B28" s="4"/>
       <c r="C28" s="5" t="s">
         <v>412</v>
       </c>
@@ -2747,8 +2735,12 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="3"/>
-      <c r="B29" s="4"/>
+      <c r="A29" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>384</v>
+      </c>
       <c r="C29" s="5" t="s">
         <v>413</v>
       </c>
@@ -2790,12 +2782,8 @@
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>383</v>
-      </c>
+      <c r="A32" s="3"/>
+      <c r="B32" s="4"/>
       <c r="C32" s="5" t="s">
         <v>416</v>
       </c>
@@ -2819,52 +2807,24 @@
         <v>477</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="3" t="s">
-        <v>376</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="3"/>
-      <c r="B36" s="4"/>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="3"/>
-      <c r="B39" s="4"/>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="3"/>
-      <c r="B40" s="4"/>
-    </row>
   </sheetData>
   <mergeCells count="16">
     <mergeCell ref="A2:A11"/>
-    <mergeCell ref="A13:A18"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A33"/>
     <mergeCell ref="B2:B11"/>
-    <mergeCell ref="B13:B18"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="B12:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
@@ -2906,7 +2866,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3051,12 +3011,8 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="3" t="s">
-        <v>490</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>498</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
         <v>510</v>
       </c>
@@ -3120,8 +3076,12 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
+      <c r="A14" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>499</v>
+      </c>
       <c r="C14" s="5" t="s">
         <v>515</v>
       </c>
@@ -3133,12 +3093,8 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="3" t="s">
-        <v>491</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>499</v>
-      </c>
+      <c r="A15" s="3"/>
+      <c r="B15" s="4"/>
       <c r="C15" s="5" t="s">
         <v>516</v>
       </c>
@@ -3150,12 +3106,8 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="3" t="s">
-        <v>491</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>499</v>
-      </c>
+      <c r="A16" s="3"/>
+      <c r="B16" s="4"/>
       <c r="C16" s="5" t="s">
         <v>517</v>
       </c>
@@ -3193,8 +3145,12 @@
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
+      <c r="A19" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>500</v>
+      </c>
       <c r="C19" s="5" t="s">
         <v>520</v>
       </c>
@@ -3236,12 +3192,8 @@
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="3" t="s">
-        <v>492</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>500</v>
-      </c>
+      <c r="A22" s="3"/>
+      <c r="B22" s="4"/>
       <c r="C22" s="5" t="s">
         <v>523</v>
       </c>
@@ -3253,8 +3205,12 @@
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="3"/>
-      <c r="B23" s="4"/>
+      <c r="A23" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>501</v>
+      </c>
       <c r="C23" s="5" t="s">
         <v>524</v>
       </c>
@@ -3266,12 +3222,8 @@
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="3" t="s">
-        <v>494</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>501</v>
-      </c>
+      <c r="A24" s="3"/>
+      <c r="B24" s="4"/>
       <c r="C24" s="5" t="s">
         <v>525</v>
       </c>
@@ -3283,12 +3235,8 @@
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="3" t="s">
-        <v>493</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>76</v>
-      </c>
+      <c r="A25" s="3"/>
+      <c r="B25" s="4"/>
       <c r="C25" s="5" t="s">
         <v>526</v>
       </c>
@@ -3300,8 +3248,12 @@
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="3"/>
-      <c r="B26" s="4"/>
+      <c r="A26" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>502</v>
+      </c>
       <c r="C26" s="5" t="s">
         <v>527</v>
       </c>
@@ -3313,12 +3265,8 @@
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="3" t="s">
-        <v>495</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>502</v>
-      </c>
+      <c r="A27" s="3"/>
+      <c r="B27" s="4"/>
       <c r="C27" s="5" t="s">
         <v>528</v>
       </c>
@@ -3330,12 +3278,8 @@
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="3" t="s">
-        <v>494</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>501</v>
-      </c>
+      <c r="A28" s="3"/>
+      <c r="B28" s="4"/>
       <c r="C28" s="5" t="s">
         <v>529</v>
       </c>
@@ -3347,8 +3291,12 @@
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="3"/>
-      <c r="B29" s="4"/>
+      <c r="A29" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>503</v>
+      </c>
       <c r="C29" s="5" t="s">
         <v>530</v>
       </c>
@@ -3373,12 +3321,8 @@
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="3" t="s">
-        <v>496</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>503</v>
-      </c>
+      <c r="A31" s="3"/>
+      <c r="B31" s="4"/>
       <c r="C31" s="5" t="s">
         <v>532</v>
       </c>
@@ -3390,12 +3334,8 @@
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="3" t="s">
-        <v>495</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>502</v>
-      </c>
+      <c r="A32" s="3"/>
+      <c r="B32" s="4"/>
       <c r="C32" s="5" t="s">
         <v>533</v>
       </c>
@@ -3405,53 +3345,25 @@
       <c r="F32" s="7" t="s">
         <v>583</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="3"/>
-      <c r="B33" s="4"/>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="3"/>
-      <c r="B34" s="4"/>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="3" t="s">
-        <v>496</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="3"/>
-      <c r="B37" s="4"/>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="3"/>
-      <c r="B38" s="4"/>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="3"/>
-      <c r="B39" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="16">
     <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A16:A20"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A29:A32"/>
     <mergeCell ref="B2:B7"/>
-    <mergeCell ref="B9:B14"/>
-    <mergeCell ref="B16:B20"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="B29:B32"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
@@ -3492,7 +3404,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3595,12 +3507,8 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
         <v>18</v>
       </c>
@@ -3653,16 +3561,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="A5:A9"/>
     <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="B5:B9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" location="best-practices_mgmt-acct_email-address"/>
@@ -3680,7 +3584,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3777,12 +3681,8 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>44</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
         <v>50</v>
       </c>
@@ -3794,8 +3694,12 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
+      <c r="A7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="C7" s="5" t="s">
         <v>51</v>
       </c>
@@ -3807,12 +3711,8 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="A8" s="3"/>
+      <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
         <v>52</v>
       </c>
@@ -3824,12 +3724,8 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
         <v>53</v>
       </c>
@@ -3839,23 +3735,15 @@
       <c r="F9" s="7" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A9"/>
     <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" location="AboutAccountAlias"/>
@@ -3873,7 +3761,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3960,12 +3848,8 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>74</v>
-      </c>
+      <c r="A5" s="3"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
         <v>81</v>
       </c>
@@ -4019,8 +3903,12 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
+      <c r="A9" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="C9" s="5" t="s">
         <v>85</v>
       </c>
@@ -4032,12 +3920,8 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>75</v>
-      </c>
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
       <c r="C10" s="5" t="s">
         <v>86</v>
       </c>
@@ -4049,12 +3933,8 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>75</v>
-      </c>
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
       <c r="C11" s="5" t="s">
         <v>87</v>
       </c>
@@ -4092,8 +3972,12 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
+      <c r="A14" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="C14" s="5" t="s">
         <v>90</v>
       </c>
@@ -4135,12 +4019,8 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>76</v>
-      </c>
+      <c r="A17" s="3"/>
+      <c r="B17" s="4"/>
       <c r="C17" s="5" t="s">
         <v>93</v>
       </c>
@@ -4153,35 +4033,19 @@
       <c r="G17" s="5" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B5:B9"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
@@ -4207,7 +4071,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4314,12 +4178,8 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>131</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
         <v>137</v>
       </c>
@@ -4334,12 +4194,8 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>131</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
         <v>138</v>
       </c>
@@ -4370,8 +4226,12 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
+      <c r="A9" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="C9" s="5" t="s">
         <v>140</v>
       </c>
@@ -4402,12 +4262,8 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>132</v>
-      </c>
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
       <c r="C11" s="5" t="s">
         <v>142</v>
       </c>
@@ -4422,12 +4278,8 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>132</v>
-      </c>
+      <c r="A12" s="3"/>
+      <c r="B12" s="4"/>
       <c r="C12" s="5" t="s">
         <v>143</v>
       </c>
@@ -4457,26 +4309,14 @@
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A13"/>
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="B9:B13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
@@ -4498,7 +4338,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4651,12 +4491,8 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>178</v>
-      </c>
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
       <c r="C10" s="5" t="s">
         <v>191</v>
       </c>
@@ -4668,12 +4504,8 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>178</v>
-      </c>
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
       <c r="C11" s="5" t="s">
         <v>192</v>
       </c>
@@ -4685,8 +4517,12 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
+      <c r="A12" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>179</v>
+      </c>
       <c r="C12" s="5" t="s">
         <v>193</v>
       </c>
@@ -4698,8 +4534,12 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
+      <c r="A13" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>180</v>
+      </c>
       <c r="C13" s="5" t="s">
         <v>194</v>
       </c>
@@ -4711,12 +4551,8 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>180</v>
-      </c>
+      <c r="A14" s="3"/>
+      <c r="B14" s="4"/>
       <c r="C14" s="5" t="s">
         <v>195</v>
       </c>
@@ -4745,12 +4581,8 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>181</v>
-      </c>
+      <c r="A16" s="3"/>
+      <c r="B16" s="4"/>
       <c r="C16" s="5" t="s">
         <v>197</v>
       </c>
@@ -4763,10 +4595,10 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="3" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>198</v>
@@ -4792,12 +4624,8 @@
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>182</v>
-      </c>
+      <c r="A19" s="3"/>
+      <c r="B19" s="4"/>
       <c r="C19" s="5" t="s">
         <v>200</v>
       </c>
@@ -4809,12 +4637,8 @@
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>181</v>
-      </c>
+      <c r="A20" s="3"/>
+      <c r="B20" s="4"/>
       <c r="C20" s="5" t="s">
         <v>201</v>
       </c>
@@ -4824,43 +4648,19 @@
       <c r="F20" s="7" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="3"/>
-      <c r="B24" s="4"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="3"/>
-      <c r="B25" s="4"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="3"/>
-      <c r="B26" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A20"/>
     <mergeCell ref="B2:B7"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B20"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
@@ -4889,7 +4689,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5005,12 +4805,8 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>239</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
         <v>246</v>
       </c>
@@ -5022,8 +4818,12 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
+      <c r="A8" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>240</v>
+      </c>
       <c r="C8" s="5" t="s">
         <v>247</v>
       </c>
@@ -5035,12 +4835,8 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>240</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
         <v>237</v>
       </c>
@@ -5052,12 +4848,8 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>240</v>
-      </c>
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
       <c r="C10" s="5" t="s">
         <v>248</v>
       </c>
@@ -5081,22 +4873,14 @@
         <v>268</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A11"/>
     <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
@@ -5116,7 +4900,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5226,12 +5010,8 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>276</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
         <v>286</v>
       </c>
@@ -5256,8 +5036,12 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
+      <c r="A9" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>277</v>
+      </c>
       <c r="C9" s="5" t="s">
         <v>288</v>
       </c>
@@ -5269,12 +5053,8 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>277</v>
-      </c>
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
       <c r="C10" s="5" t="s">
         <v>289</v>
       </c>
@@ -5287,10 +5067,10 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="3" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>290</v>
@@ -5316,12 +5096,8 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>278</v>
-      </c>
+      <c r="A13" s="3"/>
+      <c r="B13" s="4"/>
       <c r="C13" s="5" t="s">
         <v>292</v>
       </c>
@@ -5334,10 +5110,10 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="3" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>293</v>
@@ -5376,12 +5152,8 @@
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>279</v>
-      </c>
+      <c r="A17" s="3"/>
+      <c r="B17" s="4"/>
       <c r="C17" s="5" t="s">
         <v>296</v>
       </c>
@@ -5394,10 +5166,10 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="3" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>297</v>
@@ -5408,31 +5180,19 @@
       <c r="F18" s="7" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="3"/>
-      <c r="B20" s="4"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A17"/>
     <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
@@ -5459,7 +5219,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5569,12 +5329,8 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>330</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
         <v>338</v>
       </c>
@@ -5625,8 +5381,12 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
+      <c r="A11" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>331</v>
+      </c>
       <c r="C11" s="5" t="s">
         <v>342</v>
       </c>
@@ -5638,12 +5398,8 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>331</v>
-      </c>
+      <c r="A12" s="3"/>
+      <c r="B12" s="4"/>
       <c r="C12" s="5" t="s">
         <v>343</v>
       </c>
@@ -5655,12 +5411,8 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>331</v>
-      </c>
+      <c r="A13" s="3"/>
+      <c r="B13" s="4"/>
       <c r="C13" s="5" t="s">
         <v>344</v>
       </c>
@@ -5672,8 +5424,12 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
+      <c r="A14" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>332</v>
+      </c>
       <c r="C14" s="5" t="s">
         <v>345</v>
       </c>
@@ -5683,19 +5439,15 @@
       <c r="F14" s="7" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="A11:A13"/>
     <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="B11:B13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>

</xml_diff>

<commit_message>
security updates and python tool
</commit_message>
<xml_diff>
--- a/custom-lens/tools/cloud-foundations-accelerator-workbook.xlsx
+++ b/custom-lens/tools/cloud-foundations-accelerator-workbook.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="590">
   <si>
     <t>Cloud Foundations Accelerator Workbook</t>
   </si>
@@ -1631,6 +1631,9 @@
     <t>Enable cross region aggregation</t>
   </si>
   <si>
+    <t>Enable Security Hub Standard</t>
+  </si>
+  <si>
     <t xml:space="preserve">This section  is intended to provide an introduction to AWS’ approach to security, including the controls in the AWS environment and some of the products and features that AWS makes available to customers to meet your security objectives. </t>
   </si>
   <si>
@@ -1709,7 +1712,7 @@
     <t>When you use AWS Security Hub with an AWS Organizations organization, you can designate any account within the organization to be the Security Hub delegated administrator. Only the organization management account can designate Security Hub delegated administrators.  It is a best practice to delegate AWS Security Hub outside of the management account.  It is recommended to delegate Security Hub to the Security Tool account.</t>
   </si>
   <si>
-    <t>When you enable Security Hub from the console, you also have the option to enable the supported security standards.  You can configure new accounts to automatically be enabled as Security Hub member accounts.</t>
+    <t>When you enable Security Hub from the console, you also have the option to enable the supported security standards.  We recommend using the Central Configuration option of managing the organization Security Hub enabling and configuration.</t>
   </si>
   <si>
     <t>Accounts that already existed when Security Hub was enabled (and configured for automatically enabling new accounts) must still be enabled.  This can be done through the console or CLI/API.</t>
@@ -1718,6 +1721,9 @@
     <t>With cross-Region aggregation, you can aggregate findings, finding updates, insights, control compliance statuses, and security scores from multiple Regions to a single aggregation Region. You can then manage all of this data from the aggregation Region in the Security Hub administrator account.</t>
   </si>
   <si>
+    <t>A Security Hub standard is a predefined collection of rules based on regulatory frameworks and or best practices (e.g. NIST, CIS, FSBP, PCI DSS).  This allows you to measure the posture of your environment against the enable standard(s).  We recommend enabling at least 1 common standard (NIST, CIS, FSBP) and work to improve the posture of that standard.</t>
+  </si>
+  <si>
     <t>https://docs.aws.amazon.com/whitepapers/latest/introduction-aws-security/welcome.html</t>
   </si>
   <si>
@@ -1772,13 +1778,16 @@
     <t>https://docs.aws.amazon.com/securityhub/latest/userguide/designate-orgs-admin-account.html</t>
   </si>
   <si>
-    <t>https://docs.aws.amazon.com/securityhub/latest/userguide/accounts-orgs-auto-enable.html</t>
+    <t>https://docs.aws.amazon.com/securityhub/latest/userguide/central-configuration-intro.html</t>
   </si>
   <si>
     <t>https://docs.aws.amazon.com/securityhub/latest/userguide/orgs-accounts-enable.html</t>
   </si>
   <si>
     <t>https://docs.aws.amazon.com/securityhub/latest/userguide/finding-aggregation.html</t>
+  </si>
+  <si>
+    <t>https://docs.aws.amazon.com/securityhub/latest/userguide/securityhub-standards.html</t>
   </si>
   <si>
     <t xml:space="preserve">Security Pillar - AWS Well-Architected Framework : https://docs.aws.amazon.com/wellarchitected/latest/security-pillar/welcome.html; 'Best Practices for Security, Identity, &amp; Compliance' Portal : https://aws.amazon.com/architecture/security-identity-compliance/?cards-all.sort-by=item.additionalFields.sortDate&amp;cards-all.sort-order=desc&amp;awsf.content-type=*all&amp;awsf.methodology=*all; </t>
@@ -2287,7 +2296,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2496,12 +2505,8 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>380</v>
-      </c>
+      <c r="A13" s="3"/>
+      <c r="B13" s="4"/>
       <c r="C13" s="5" t="s">
         <v>398</v>
       </c>
@@ -2580,8 +2585,12 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
+      <c r="A18" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>381</v>
+      </c>
       <c r="C18" s="5" t="s">
         <v>403</v>
       </c>
@@ -2593,12 +2602,8 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>381</v>
-      </c>
+      <c r="A19" s="3"/>
+      <c r="B19" s="4"/>
       <c r="C19" s="5" t="s">
         <v>404</v>
       </c>
@@ -2611,10 +2616,10 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="3" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>405</v>
@@ -2640,12 +2645,8 @@
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="3" t="s">
-        <v>374</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>382</v>
-      </c>
+      <c r="A22" s="3"/>
+      <c r="B22" s="4"/>
       <c r="C22" s="5" t="s">
         <v>407</v>
       </c>
@@ -2657,12 +2658,8 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="3" t="s">
-        <v>374</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>382</v>
-      </c>
+      <c r="A23" s="3"/>
+      <c r="B23" s="4"/>
       <c r="C23" s="5" t="s">
         <v>408</v>
       </c>
@@ -2674,8 +2671,12 @@
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="3"/>
-      <c r="B24" s="4"/>
+      <c r="A24" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>383</v>
+      </c>
       <c r="C24" s="5" t="s">
         <v>409</v>
       </c>
@@ -2733,12 +2734,8 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>383</v>
-      </c>
+      <c r="A28" s="3"/>
+      <c r="B28" s="4"/>
       <c r="C28" s="5" t="s">
         <v>413</v>
       </c>
@@ -2750,8 +2747,12 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="3"/>
-      <c r="B29" s="4"/>
+      <c r="A29" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>385</v>
+      </c>
       <c r="C29" s="5" t="s">
         <v>414</v>
       </c>
@@ -2793,12 +2794,8 @@
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="3" t="s">
-        <v>376</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>384</v>
-      </c>
+      <c r="A32" s="3"/>
+      <c r="B32" s="4"/>
       <c r="C32" s="5" t="s">
         <v>417</v>
       </c>
@@ -2822,52 +2819,24 @@
         <v>478</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="3"/>
-      <c r="B36" s="4"/>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="3"/>
-      <c r="B39" s="4"/>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="3"/>
-      <c r="B40" s="4"/>
-    </row>
   </sheetData>
   <mergeCells count="16">
     <mergeCell ref="A2:A11"/>
-    <mergeCell ref="A13:A18"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A33"/>
     <mergeCell ref="B2:B11"/>
-    <mergeCell ref="B13:B18"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="B12:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
@@ -2909,7 +2878,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2959,13 +2928,13 @@
         <v>505</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -2975,10 +2944,10 @@
         <v>506</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2991,7 +2960,7 @@
         <v>503</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -3001,10 +2970,10 @@
         <v>340</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -3014,10 +2983,10 @@
         <v>508</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -3027,13 +2996,13 @@
         <v>509</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>586</v>
+        <v>589</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -3047,27 +3016,23 @@
         <v>510</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="3" t="s">
-        <v>491</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>499</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
         <v>511</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -3077,10 +3042,10 @@
         <v>512</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -3090,10 +3055,10 @@
         <v>513</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -3103,10 +3068,10 @@
         <v>514</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -3116,57 +3081,53 @@
         <v>515</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
+      <c r="A14" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>500</v>
+      </c>
       <c r="C14" s="5" t="s">
         <v>516</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="3" t="s">
-        <v>492</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>500</v>
-      </c>
+      <c r="A15" s="3"/>
+      <c r="B15" s="4"/>
       <c r="C15" s="5" t="s">
         <v>517</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="3" t="s">
-        <v>492</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>500</v>
-      </c>
+      <c r="A16" s="3"/>
+      <c r="B16" s="4"/>
       <c r="C16" s="5" t="s">
         <v>518</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -3176,10 +3137,10 @@
         <v>519</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -3189,20 +3150,24 @@
         <v>520</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
+      <c r="A19" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>501</v>
+      </c>
       <c r="C19" s="5" t="s">
         <v>521</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>121</v>
@@ -3215,7 +3180,7 @@
         <v>522</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>121</v>
@@ -3232,134 +3197,126 @@
         <v>523</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="3" t="s">
-        <v>493</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>501</v>
-      </c>
+      <c r="A22" s="3"/>
+      <c r="B22" s="4"/>
       <c r="C22" s="5" t="s">
         <v>524</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="3"/>
-      <c r="B23" s="4"/>
+      <c r="A23" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>502</v>
+      </c>
       <c r="C23" s="5" t="s">
         <v>525</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="3" t="s">
-        <v>495</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>502</v>
-      </c>
+      <c r="A24" s="3"/>
+      <c r="B24" s="4"/>
       <c r="C24" s="5" t="s">
         <v>526</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="3" t="s">
-        <v>494</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>77</v>
-      </c>
+      <c r="A25" s="3"/>
+      <c r="B25" s="4"/>
       <c r="C25" s="5" t="s">
         <v>527</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="3"/>
-      <c r="B26" s="4"/>
+      <c r="A26" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>503</v>
+      </c>
       <c r="C26" s="5" t="s">
         <v>528</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="3" t="s">
-        <v>496</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>503</v>
-      </c>
+      <c r="A27" s="3"/>
+      <c r="B27" s="4"/>
       <c r="C27" s="5" t="s">
         <v>529</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="3" t="s">
-        <v>495</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>502</v>
-      </c>
+      <c r="A28" s="3"/>
+      <c r="B28" s="4"/>
       <c r="C28" s="5" t="s">
         <v>530</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="3"/>
-      <c r="B29" s="4"/>
+      <c r="A29" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>504</v>
+      </c>
       <c r="C29" s="5" t="s">
         <v>531</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -3369,92 +3326,69 @@
         <v>532</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="3" t="s">
-        <v>497</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>504</v>
-      </c>
+      <c r="A31" s="3"/>
+      <c r="B31" s="4"/>
       <c r="C31" s="5" t="s">
         <v>533</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="3" t="s">
-        <v>496</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>503</v>
-      </c>
+      <c r="A32" s="3"/>
+      <c r="B32" s="4"/>
       <c r="C32" s="5" t="s">
         <v>534</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="3"/>
-      <c r="B34" s="4"/>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="3" t="s">
-        <v>497</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="3"/>
-      <c r="B37" s="4"/>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="3"/>
-      <c r="B38" s="4"/>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="3"/>
-      <c r="B39" s="4"/>
+      <c r="C33" s="5" t="s">
+        <v>535</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>565</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>587</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="16">
     <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A16:A20"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A29:A33"/>
     <mergeCell ref="B2:B7"/>
-    <mergeCell ref="B9:B14"/>
-    <mergeCell ref="B16:B20"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="B29:B33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
@@ -3488,6 +3422,7 @@
     <hyperlink ref="F30" r:id="rId29"/>
     <hyperlink ref="F31" r:id="rId30"/>
     <hyperlink ref="F32" r:id="rId31"/>
+    <hyperlink ref="F33" r:id="rId32"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3495,7 +3430,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3598,12 +3533,8 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
         <v>19</v>
       </c>
@@ -3656,16 +3587,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="A5:A9"/>
     <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="B5:B9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" location="best-practices_mgmt-acct_email-address"/>
@@ -3683,7 +3610,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3780,12 +3707,8 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
         <v>51</v>
       </c>
@@ -3797,8 +3720,12 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
+      <c r="A7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="C7" s="5" t="s">
         <v>52</v>
       </c>
@@ -3810,12 +3737,8 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>46</v>
-      </c>
+      <c r="A8" s="3"/>
+      <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
         <v>53</v>
       </c>
@@ -3827,12 +3750,8 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>46</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
         <v>54</v>
       </c>
@@ -3842,23 +3761,15 @@
       <c r="F9" s="7" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A9"/>
     <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" location="AboutAccountAlias"/>
@@ -3876,7 +3787,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3963,12 +3874,8 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>75</v>
-      </c>
+      <c r="A5" s="3"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
         <v>82</v>
       </c>
@@ -4022,8 +3929,12 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
+      <c r="A9" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="C9" s="5" t="s">
         <v>86</v>
       </c>
@@ -4035,12 +3946,8 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>76</v>
-      </c>
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
       <c r="C10" s="5" t="s">
         <v>87</v>
       </c>
@@ -4052,12 +3959,8 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>76</v>
-      </c>
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
       <c r="C11" s="5" t="s">
         <v>88</v>
       </c>
@@ -4095,8 +3998,12 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
+      <c r="A14" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="C14" s="5" t="s">
         <v>91</v>
       </c>
@@ -4138,12 +4045,8 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>77</v>
-      </c>
+      <c r="A17" s="3"/>
+      <c r="B17" s="4"/>
       <c r="C17" s="5" t="s">
         <v>94</v>
       </c>
@@ -4156,35 +4059,19 @@
       <c r="G17" s="5" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B5:B9"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
@@ -4210,7 +4097,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4317,12 +4204,8 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>132</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
         <v>138</v>
       </c>
@@ -4337,12 +4220,8 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>132</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
         <v>139</v>
       </c>
@@ -4373,8 +4252,12 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
+      <c r="A9" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>133</v>
+      </c>
       <c r="C9" s="5" t="s">
         <v>141</v>
       </c>
@@ -4405,12 +4288,8 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>133</v>
-      </c>
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
       <c r="C11" s="5" t="s">
         <v>143</v>
       </c>
@@ -4425,12 +4304,8 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>133</v>
-      </c>
+      <c r="A12" s="3"/>
+      <c r="B12" s="4"/>
       <c r="C12" s="5" t="s">
         <v>144</v>
       </c>
@@ -4460,26 +4335,14 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A13"/>
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="B9:B13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
@@ -4501,7 +4364,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4654,12 +4517,8 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>179</v>
-      </c>
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
       <c r="C10" s="5" t="s">
         <v>192</v>
       </c>
@@ -4671,12 +4530,8 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>179</v>
-      </c>
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
       <c r="C11" s="5" t="s">
         <v>193</v>
       </c>
@@ -4688,8 +4543,12 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
+      <c r="A12" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>180</v>
+      </c>
       <c r="C12" s="5" t="s">
         <v>194</v>
       </c>
@@ -4701,8 +4560,12 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
+      <c r="A13" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>181</v>
+      </c>
       <c r="C13" s="5" t="s">
         <v>195</v>
       </c>
@@ -4714,12 +4577,8 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>181</v>
-      </c>
+      <c r="A14" s="3"/>
+      <c r="B14" s="4"/>
       <c r="C14" s="5" t="s">
         <v>196</v>
       </c>
@@ -4748,12 +4607,8 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>182</v>
-      </c>
+      <c r="A16" s="3"/>
+      <c r="B16" s="4"/>
       <c r="C16" s="5" t="s">
         <v>198</v>
       </c>
@@ -4766,10 +4621,10 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>199</v>
@@ -4795,12 +4650,8 @@
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>183</v>
-      </c>
+      <c r="A19" s="3"/>
+      <c r="B19" s="4"/>
       <c r="C19" s="5" t="s">
         <v>201</v>
       </c>
@@ -4812,12 +4663,8 @@
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>182</v>
-      </c>
+      <c r="A20" s="3"/>
+      <c r="B20" s="4"/>
       <c r="C20" s="5" t="s">
         <v>202</v>
       </c>
@@ -4827,43 +4674,19 @@
       <c r="F20" s="7" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="3"/>
-      <c r="B24" s="4"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="3"/>
-      <c r="B25" s="4"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="3"/>
-      <c r="B26" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A20"/>
     <mergeCell ref="B2:B7"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B20"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
@@ -4892,7 +4715,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5008,12 +4831,8 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>240</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
         <v>247</v>
       </c>
@@ -5025,8 +4844,12 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
+      <c r="A8" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>241</v>
+      </c>
       <c r="C8" s="5" t="s">
         <v>248</v>
       </c>
@@ -5038,12 +4861,8 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>241</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
         <v>238</v>
       </c>
@@ -5055,12 +4874,8 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>241</v>
-      </c>
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
       <c r="C10" s="5" t="s">
         <v>249</v>
       </c>
@@ -5084,22 +4899,14 @@
         <v>269</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A11"/>
     <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
@@ -5119,7 +4926,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5229,12 +5036,8 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>277</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
         <v>287</v>
       </c>
@@ -5259,8 +5062,12 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
+      <c r="A9" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>278</v>
+      </c>
       <c r="C9" s="5" t="s">
         <v>289</v>
       </c>
@@ -5272,12 +5079,8 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>278</v>
-      </c>
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
       <c r="C10" s="5" t="s">
         <v>290</v>
       </c>
@@ -5290,10 +5093,10 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="3" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>291</v>
@@ -5319,12 +5122,8 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>279</v>
-      </c>
+      <c r="A13" s="3"/>
+      <c r="B13" s="4"/>
       <c r="C13" s="5" t="s">
         <v>293</v>
       </c>
@@ -5337,10 +5136,10 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="3" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>294</v>
@@ -5379,12 +5178,8 @@
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>280</v>
-      </c>
+      <c r="A17" s="3"/>
+      <c r="B17" s="4"/>
       <c r="C17" s="5" t="s">
         <v>297</v>
       </c>
@@ -5397,10 +5192,10 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="3" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>298</v>
@@ -5411,31 +5206,19 @@
       <c r="F18" s="7" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="3"/>
-      <c r="B20" s="4"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A17"/>
     <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
@@ -5462,7 +5245,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5572,12 +5355,8 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>331</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
         <v>339</v>
       </c>
@@ -5628,8 +5407,12 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
+      <c r="A11" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>332</v>
+      </c>
       <c r="C11" s="5" t="s">
         <v>343</v>
       </c>
@@ -5641,12 +5424,8 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>332</v>
-      </c>
+      <c r="A12" s="3"/>
+      <c r="B12" s="4"/>
       <c r="C12" s="5" t="s">
         <v>344</v>
       </c>
@@ -5658,12 +5437,8 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>332</v>
-      </c>
+      <c r="A13" s="3"/>
+      <c r="B13" s="4"/>
       <c r="C13" s="5" t="s">
         <v>345</v>
       </c>
@@ -5675,8 +5450,12 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
+      <c r="A14" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>333</v>
+      </c>
       <c r="C14" s="5" t="s">
         <v>346</v>
       </c>
@@ -5686,19 +5465,15 @@
       <c r="F14" s="7" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="A11:A13"/>
     <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="B11:B13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>

</xml_diff>

<commit_message>
feat: Lens updates (#78)
</commit_message>
<xml_diff>
--- a/custom-lens/tools/cloud-foundations-accelerator-workbook.xlsx
+++ b/custom-lens/tools/cloud-foundations-accelerator-workbook.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="589">
   <si>
     <t>Cloud Foundations Accelerator Workbook</t>
   </si>
@@ -695,7 +695,7 @@
     <t>https://docs.aws.amazon.com/IAM/latest/UserGuide/introduction.html</t>
   </si>
   <si>
-    <t>https://docs.aws.amazon.com/IAM/latest/UserGuide/introduction_access-management.html</t>
+    <t>https://docs.aws.amazon.com/IAM/latest/UserGuide/id_root-user.html</t>
   </si>
   <si>
     <t>https://docs.aws.amazon.com/IAM/latest/UserGuide/access_policies_identity-vs-resource.html</t>
@@ -719,9 +719,6 @@
     <t>https://docs.aws.amazon.com/singlesignon/latest/userguide/howtochangeURL.html</t>
   </si>
   <si>
-    <t>https://docs.aws.amazon.com/IAM/latest/UserGuide/id_root-user.html</t>
-  </si>
-  <si>
     <t>https://docs.aws.amazon.com/controltower/latest/userguide/provision-as-end-user.html</t>
   </si>
   <si>
@@ -1631,6 +1628,9 @@
     <t>Enable cross region aggregation</t>
   </si>
   <si>
+    <t>Enable Security Hub Standard</t>
+  </si>
+  <si>
     <t xml:space="preserve">This section  is intended to provide an introduction to AWS’ approach to security, including the controls in the AWS environment and some of the products and features that AWS makes available to customers to meet your security objectives. </t>
   </si>
   <si>
@@ -1709,7 +1709,7 @@
     <t>When you use AWS Security Hub with an AWS Organizations organization, you can designate any account within the organization to be the Security Hub delegated administrator. Only the organization management account can designate Security Hub delegated administrators.  It is a best practice to delegate AWS Security Hub outside of the management account.  It is recommended to delegate Security Hub to the Security Tool account.</t>
   </si>
   <si>
-    <t>When you enable Security Hub from the console, you also have the option to enable the supported security standards.  You can configure new accounts to automatically be enabled as Security Hub member accounts.</t>
+    <t>When you enable Security Hub from the console, you also have the option to enable the supported security standards.  We recommend using the Central Configuration option of managing the organization Security Hub enabling and configuration.</t>
   </si>
   <si>
     <t>Accounts that already existed when Security Hub was enabled (and configured for automatically enabling new accounts) must still be enabled.  This can be done through the console or CLI/API.</t>
@@ -1718,6 +1718,9 @@
     <t>With cross-Region aggregation, you can aggregate findings, finding updates, insights, control compliance statuses, and security scores from multiple Regions to a single aggregation Region. You can then manage all of this data from the aggregation Region in the Security Hub administrator account.</t>
   </si>
   <si>
+    <t>A Security Hub standard is a predefined collection of rules based on regulatory frameworks and or best practices (e.g. NIST, CIS, FSBP, PCI DSS).  This allows you to measure the posture of your environment against the enable standard(s).  We recommend enabling at least 1 common standard (NIST, CIS, FSBP) and work to improve the posture of that standard.</t>
+  </si>
+  <si>
     <t>https://docs.aws.amazon.com/whitepapers/latest/introduction-aws-security/welcome.html</t>
   </si>
   <si>
@@ -1772,13 +1775,16 @@
     <t>https://docs.aws.amazon.com/securityhub/latest/userguide/designate-orgs-admin-account.html</t>
   </si>
   <si>
-    <t>https://docs.aws.amazon.com/securityhub/latest/userguide/accounts-orgs-auto-enable.html</t>
+    <t>https://docs.aws.amazon.com/securityhub/latest/userguide/central-configuration-intro.html</t>
   </si>
   <si>
     <t>https://docs.aws.amazon.com/securityhub/latest/userguide/orgs-accounts-enable.html</t>
   </si>
   <si>
     <t>https://docs.aws.amazon.com/securityhub/latest/userguide/finding-aggregation.html</t>
+  </si>
+  <si>
+    <t>https://docs.aws.amazon.com/securityhub/latest/userguide/securityhub-standards.html</t>
   </si>
   <si>
     <t xml:space="preserve">Security Pillar - AWS Well-Architected Framework : https://docs.aws.amazon.com/wellarchitected/latest/security-pillar/welcome.html; 'Best Practices for Security, Identity, &amp; Compliance' Portal : https://aws.amazon.com/architecture/security-identity-compliance/?cards-all.sort-by=item.additionalFields.sortDate&amp;cards-all.sort-order=desc&amp;awsf.content-type=*all&amp;awsf.methodology=*all; </t>
@@ -2287,7 +2293,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2331,87 +2337,87 @@
         <v>69</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>161</v>
@@ -2421,192 +2427,188 @@
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C12" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>457</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="3"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="5" t="s">
         <v>397</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>428</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F13" s="7" t="s">
         <v>458</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G13" s="5" t="s">
         <v>484</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>380</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>398</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>429</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>459</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
       <c r="C17" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>462</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>402</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E18" s="5" t="s">
         <v>433</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F18" s="7" t="s">
         <v>463</v>
       </c>
-      <c r="G17" s="5" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="5" t="s">
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="3"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="5" t="s">
         <v>403</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E19" s="5" t="s">
         <v>434</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F19" s="7" t="s">
         <v>464</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>381</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>404</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>435</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -2617,257 +2619,221 @@
         <v>381</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
       <c r="C21" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="3"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="5" t="s">
         <v>406</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E22" s="5" t="s">
         <v>437</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F22" s="7" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="3" t="s">
+    <row r="23" spans="1:7">
+      <c r="A23" s="3"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="3" t="s">
         <v>374</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>407</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>438</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="3" t="s">
-        <v>374</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="C23" s="5" t="s">
+      <c r="C24" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E24" s="5" t="s">
         <v>439</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F24" s="7" t="s">
         <v>469</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="3"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="5" t="s">
-        <v>409</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>440</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="3"/>
       <c r="B25" s="4"/>
       <c r="C25" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
       <c r="C26" s="5" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="3"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>412</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>443</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="C28" s="5" t="s">
+      <c r="C29" s="5" t="s">
         <v>413</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E29" s="5" t="s">
         <v>444</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F29" s="7" t="s">
         <v>474</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="3"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="5" t="s">
-        <v>414</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>445</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
       <c r="C30" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C31" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="3"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="5" t="s">
         <v>416</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E32" s="5" t="s">
         <v>447</v>
       </c>
-      <c r="F31" s="7" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="3" t="s">
-        <v>376</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>417</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>448</v>
-      </c>
       <c r="F32" s="7" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
       <c r="C33" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="3"/>
-      <c r="B36" s="4"/>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="3"/>
-      <c r="B39" s="4"/>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="3"/>
-      <c r="B40" s="4"/>
+        <v>477</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="16">
     <mergeCell ref="A2:A11"/>
-    <mergeCell ref="A13:A18"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A33"/>
     <mergeCell ref="B2:B11"/>
-    <mergeCell ref="B13:B18"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="B12:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
@@ -2909,7 +2875,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2953,253 +2919,249 @@
         <v>69</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>535</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>536</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>537</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>538</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>539</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="3" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>540</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="3" t="s">
-        <v>491</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>499</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>541</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="5" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>542</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>543</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="C12" s="5" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>544</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="5" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>545</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
+      <c r="A14" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>499</v>
+      </c>
       <c r="C14" s="5" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>546</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="3" t="s">
-        <v>492</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>500</v>
-      </c>
+      <c r="A15" s="3"/>
+      <c r="B15" s="4"/>
       <c r="C15" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>547</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="3" t="s">
-        <v>492</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>500</v>
-      </c>
+      <c r="A16" s="3"/>
+      <c r="B16" s="4"/>
       <c r="C16" s="5" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>544</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
       <c r="C17" s="5" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>548</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="3"/>
       <c r="B18" s="4"/>
       <c r="C18" s="5" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>549</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
+      <c r="A19" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>500</v>
+      </c>
       <c r="C19" s="5" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>550</v>
@@ -3212,7 +3174,7 @@
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>551</v>
@@ -3223,13 +3185,13 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>77</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>552</v>
@@ -3239,14 +3201,10 @@
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="3" t="s">
-        <v>493</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>501</v>
-      </c>
+      <c r="A22" s="3"/>
+      <c r="B22" s="4"/>
       <c r="C22" s="5" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>553</v>
@@ -3256,10 +3214,14 @@
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="3"/>
-      <c r="B23" s="4"/>
+      <c r="A23" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>501</v>
+      </c>
       <c r="C23" s="5" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>554</v>
@@ -3269,192 +3231,161 @@
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="3" t="s">
-        <v>495</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>502</v>
-      </c>
+      <c r="A24" s="3"/>
+      <c r="B24" s="4"/>
       <c r="C24" s="5" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>555</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="3" t="s">
-        <v>494</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>77</v>
-      </c>
+      <c r="A25" s="3"/>
+      <c r="B25" s="4"/>
       <c r="C25" s="5" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>556</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="3"/>
-      <c r="B26" s="4"/>
+      <c r="A26" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>502</v>
+      </c>
       <c r="C26" s="5" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>557</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="3" t="s">
-        <v>496</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>503</v>
-      </c>
+      <c r="A27" s="3"/>
+      <c r="B27" s="4"/>
       <c r="C27" s="5" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>558</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="3" t="s">
-        <v>495</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>502</v>
-      </c>
+      <c r="A28" s="3"/>
+      <c r="B28" s="4"/>
       <c r="C28" s="5" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>559</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="3"/>
-      <c r="B29" s="4"/>
+      <c r="A29" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>503</v>
+      </c>
       <c r="C29" s="5" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>560</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
       <c r="C30" s="5" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>561</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="3" t="s">
-        <v>497</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>504</v>
-      </c>
+      <c r="A31" s="3"/>
+      <c r="B31" s="4"/>
       <c r="C31" s="5" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>562</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="3" t="s">
-        <v>496</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>503</v>
-      </c>
+      <c r="A32" s="3"/>
+      <c r="B32" s="4"/>
       <c r="C32" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>563</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="3"/>
-      <c r="B34" s="4"/>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="3" t="s">
-        <v>497</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="3"/>
-      <c r="B37" s="4"/>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="3"/>
-      <c r="B38" s="4"/>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="3"/>
-      <c r="B39" s="4"/>
+      <c r="C33" s="5" t="s">
+        <v>534</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>564</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>586</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="16">
     <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A16:A20"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A29:A33"/>
     <mergeCell ref="B2:B7"/>
-    <mergeCell ref="B9:B14"/>
-    <mergeCell ref="B16:B20"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="B29:B33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
@@ -3488,6 +3419,7 @@
     <hyperlink ref="F30" r:id="rId29"/>
     <hyperlink ref="F31" r:id="rId30"/>
     <hyperlink ref="F32" r:id="rId31"/>
+    <hyperlink ref="F33" r:id="rId32"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3495,7 +3427,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3598,12 +3530,8 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
         <v>19</v>
       </c>
@@ -3656,16 +3584,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="A5:A9"/>
     <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="B5:B9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" location="best-practices_mgmt-acct_email-address"/>
@@ -3683,7 +3607,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3780,12 +3704,8 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
         <v>51</v>
       </c>
@@ -3797,8 +3717,12 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
+      <c r="A7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="C7" s="5" t="s">
         <v>52</v>
       </c>
@@ -3810,12 +3734,8 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>46</v>
-      </c>
+      <c r="A8" s="3"/>
+      <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
         <v>53</v>
       </c>
@@ -3827,12 +3747,8 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>46</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
         <v>54</v>
       </c>
@@ -3842,23 +3758,15 @@
       <c r="F9" s="7" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A9"/>
     <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" location="AboutAccountAlias"/>
@@ -3876,7 +3784,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3963,12 +3871,8 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>75</v>
-      </c>
+      <c r="A5" s="3"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
         <v>82</v>
       </c>
@@ -4022,8 +3926,12 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
+      <c r="A9" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="C9" s="5" t="s">
         <v>86</v>
       </c>
@@ -4035,12 +3943,8 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>76</v>
-      </c>
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
       <c r="C10" s="5" t="s">
         <v>87</v>
       </c>
@@ -4052,12 +3956,8 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>76</v>
-      </c>
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
       <c r="C11" s="5" t="s">
         <v>88</v>
       </c>
@@ -4095,8 +3995,12 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
+      <c r="A14" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="C14" s="5" t="s">
         <v>91</v>
       </c>
@@ -4138,12 +4042,8 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>77</v>
-      </c>
+      <c r="A17" s="3"/>
+      <c r="B17" s="4"/>
       <c r="C17" s="5" t="s">
         <v>94</v>
       </c>
@@ -4156,35 +4056,19 @@
       <c r="G17" s="5" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B5:B9"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
@@ -4210,7 +4094,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4317,12 +4201,8 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>132</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
         <v>138</v>
       </c>
@@ -4337,12 +4217,8 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>132</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
         <v>139</v>
       </c>
@@ -4373,8 +4249,12 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
+      <c r="A9" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>133</v>
+      </c>
       <c r="C9" s="5" t="s">
         <v>141</v>
       </c>
@@ -4405,12 +4285,8 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>133</v>
-      </c>
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
       <c r="C11" s="5" t="s">
         <v>143</v>
       </c>
@@ -4425,12 +4301,8 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>133</v>
-      </c>
+      <c r="A12" s="3"/>
+      <c r="B12" s="4"/>
       <c r="C12" s="5" t="s">
         <v>144</v>
       </c>
@@ -4460,26 +4332,14 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A13"/>
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="B9:B13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
@@ -4501,7 +4361,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4654,12 +4514,8 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>179</v>
-      </c>
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
       <c r="C10" s="5" t="s">
         <v>192</v>
       </c>
@@ -4671,12 +4527,8 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>179</v>
-      </c>
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
       <c r="C11" s="5" t="s">
         <v>193</v>
       </c>
@@ -4688,8 +4540,12 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
+      <c r="A12" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>180</v>
+      </c>
       <c r="C12" s="5" t="s">
         <v>194</v>
       </c>
@@ -4697,12 +4553,16 @@
         <v>213</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
+      <c r="A13" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>181</v>
+      </c>
       <c r="C13" s="5" t="s">
         <v>195</v>
       </c>
@@ -4710,16 +4570,12 @@
         <v>214</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>181</v>
-      </c>
+      <c r="A14" s="3"/>
+      <c r="B14" s="4"/>
       <c r="C14" s="5" t="s">
         <v>196</v>
       </c>
@@ -4727,7 +4583,7 @@
         <v>215</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -4744,16 +4600,12 @@
         <v>216</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>182</v>
-      </c>
+      <c r="A16" s="3"/>
+      <c r="B16" s="4"/>
       <c r="C16" s="5" t="s">
         <v>198</v>
       </c>
@@ -4761,15 +4613,15 @@
         <v>217</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>199</v>
@@ -4795,12 +4647,8 @@
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>183</v>
-      </c>
+      <c r="A19" s="3"/>
+      <c r="B19" s="4"/>
       <c r="C19" s="5" t="s">
         <v>201</v>
       </c>
@@ -4808,16 +4656,12 @@
         <v>220</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>182</v>
-      </c>
+      <c r="A20" s="3"/>
+      <c r="B20" s="4"/>
       <c r="C20" s="5" t="s">
         <v>202</v>
       </c>
@@ -4825,45 +4669,21 @@
         <v>221</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="3"/>
-      <c r="B24" s="4"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="3"/>
-      <c r="B25" s="4"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="3"/>
-      <c r="B26" s="4"/>
+        <v>235</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A20"/>
     <mergeCell ref="B2:B7"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B20"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
@@ -4892,7 +4712,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4936,170 +4756,154 @@
         <v>69</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="F6" s="7" t="s">
+      <c r="C8" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="3" t="s">
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5" t="s">
+      <c r="E9" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="E9" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F10" s="7" t="s">
         <v>267</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
+        <v>268</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A11"/>
     <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
@@ -5119,7 +4923,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5160,132 +4964,128 @@
         <v>69</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>304</v>
-      </c>
       <c r="F7" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5" t="s">
+      <c r="F9" s="7" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>306</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>307</v>
-      </c>
       <c r="F10" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -5296,43 +5096,39 @@
         <v>278</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="C12" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="3"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F13" s="7" t="s">
         <v>322</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -5343,56 +5139,52 @@
         <v>279</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="3"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>313</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F17" s="7" t="s">
         <v>324</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -5403,39 +5195,27 @@
         <v>280</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="3"/>
-      <c r="B20" s="4"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
+        <v>325</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A17"/>
     <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
@@ -5462,7 +5242,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5503,202 +5283,194 @@
         <v>69</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="5" t="s">
         <v>338</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F7" s="7" t="s">
         <v>363</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>339</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>352</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>342</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F11" s="7" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="5" t="s">
+    <row r="12" spans="1:7">
+      <c r="A12" s="3"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="5" t="s">
         <v>343</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E12" s="5" t="s">
         <v>356</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F12" s="7" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="3" t="s">
+    <row r="13" spans="1:7">
+      <c r="A13" s="3"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B14" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>357</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="C13" s="5" t="s">
+      <c r="C14" s="5" t="s">
         <v>345</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F14" s="7" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="5" t="s">
-        <v>346</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>359</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="A11:A13"/>
     <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="B11:B13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>

</xml_diff>